<commit_message>
Output auxiliary files in fmudesign init
</commit_message>
<xml_diff>
--- a/src/semeio/fmudesign/examples/ex1_onebyone_rms_repeat.xlsx
+++ b/src/semeio/fmudesign/examples/ex1_onebyone_rms_repeat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\fmu\users\tral\fmu-utils\github\fmu-tools\tests\data\sensitivities\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Appl\github\semeio\src\semeio\fmudesign\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759DF6AA-3164-44B8-BF63-B0A458DF9502}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B583273E-17FC-42C5-8A9C-B486D915D811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3225" yWindow="2175" windowWidth="21600" windowHeight="9450" tabRatio="990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" r:id="rId1"/>
@@ -21,94 +21,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Trine Alsos</author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{8E1058AB-4A5B-4437-84AF-48DF2B2D7649}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Specifies that this is a setup for a onebyone design. </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{F23FB59F-9F63-447D-A084-EF6B6518D7A5}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Number of repeated seeds per sensitivity/sensitivity  case.
-This is overridden if number of realisations is specified in the numreal column in designinput.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{4DB46DC7-81A0-484E-8599-655EC3B70562}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Alternatives:
-- default: gives RMS_SEED numbers 1000, 1001, 1002, 1003,…
-- None (seed number is not added as parameter in spreadsheet)
-- filename for file with list of seeds (in same folder)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{B110C137-F7B3-49F6-AF79-113D17B32073}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Alternatives:
-- None
-- name of sheet in this workbook with background parameters
-- Name of external file with background parameters. Must end with .xlsx or .csv and be readable as pandas dataframe with parameter names as column headers. Path is relaitve to where script is run from.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{30537938-8759-4473-B808-D1F8CCFBD774}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(optional)
-Alternatives:
-- Integer 
-- None</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t>designtype</t>
   </si>
@@ -248,19 +162,7 @@
     <t>base</t>
   </si>
   <si>
-    <t>PARAM1</t>
-  </si>
-  <si>
-    <t>PARAM2</t>
-  </si>
-  <si>
     <t>0.1</t>
-  </si>
-  <si>
-    <t>PARAM3</t>
-  </si>
-  <si>
-    <t>PARAM4</t>
   </si>
   <si>
     <t>rms_seeds</t>
@@ -273,7 +175,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -288,12 +190,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1001,10 +897,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1039,13 +935,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1066,13 +962,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1095,14 +991,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1125,13 +1021,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1158,9 +1054,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1173,7 +1069,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1186,8 +1082,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1208,20 +1104,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1235,11 +1131,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1328,9 +1219,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1368,7 +1259,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1474,7 +1365,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1616,24 +1507,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="111"/>
+    <col min="2" max="2" width="10" style="2"/>
     <col min="3" max="3" width="77.85546875"/>
     <col min="4" max="1025" width="8.7109375"/>
   </cols>
@@ -1656,7 +1547,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -1666,16 +1557,16 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="111" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>48</v>
+      </c>
+      <c r="B5" s="2">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1685,7 +1576,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1694,23 +1584,24 @@
   <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D13" activeCellId="1" sqref="A5:B5 D13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875"/>
-    <col min="2" max="2" width="8.42578125"/>
-    <col min="3" max="3" width="8.28515625"/>
-    <col min="4" max="4" width="15.140625"/>
-    <col min="5" max="5" width="10" style="2"/>
-    <col min="6" max="6" width="11.85546875" style="2"/>
-    <col min="7" max="7" width="9.85546875" style="2"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="2"/>
     <col min="9" max="9" width="11.85546875"/>
-    <col min="10" max="10" width="11.5703125" style="2"/>
-    <col min="11" max="14" width="11.85546875" style="2"/>
-    <col min="15" max="17" width="11.85546875"/>
+    <col min="10" max="13" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875"/>
     <col min="18" max="19" width="8.7109375"/>
     <col min="20" max="20" width="9.85546875"/>
     <col min="21" max="21" width="8.7109375"/>
@@ -1975,10 +1866,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1997,7 +1888,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="109" t="s">
+      <c r="A2" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="2">
@@ -2005,7 +1896,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="109" t="s">
+      <c r="A3" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="2">
@@ -2013,7 +1904,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="109" t="s">
+      <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2021,7 +1912,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="109" t="s">
+      <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="2">
@@ -2029,7 +1920,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="109" t="s">
+      <c r="A6" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="2">
@@ -2037,7 +1928,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="109" t="s">
+      <c r="A7" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="2">
@@ -2045,43 +1936,11 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="109" t="s">
+      <c r="A8" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="110" t="s">
         <v>46</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="110" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="110" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="110" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean up Excel files: remove comments, prettify formatting
</commit_message>
<xml_diff>
--- a/src/semeio/fmudesign/examples/ex1_onebyone_rms_repeat.xlsx
+++ b/src/semeio/fmudesign/examples/ex1_onebyone_rms_repeat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Appl\github\semeio\src\semeio\fmudesign\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B583273E-17FC-42C5-8A9C-B486D915D811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A017934A-1643-42F0-8E5F-61F919C38CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" r:id="rId1"/>
@@ -1583,8 +1583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1868,7 +1868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>